<commit_message>
Working on removing photos
</commit_message>
<xml_diff>
--- a/Quizzes/Graded/Grades.xlsx
+++ b/Quizzes/Graded/Grades.xlsx
@@ -393,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL24"/>
+  <dimension ref="A1:AL25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+      <selection activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2620,10 +2620,7 @@
         <f t="shared" si="27"/>
         <v>0.62333333333333329</v>
       </c>
-      <c r="S21" s="4" t="e">
-        <f t="shared" si="27"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="S21" s="4"/>
       <c r="T21" s="6">
         <f t="shared" si="27"/>
         <v>0.71333333333333337</v>
@@ -2699,6 +2696,45 @@
       <c r="A24" s="7" t="str">
         <f>CONCATENATE(IF(AA23&lt;0.05,"","not "),"statistically significant")</f>
         <v>not statistically significant</v>
+      </c>
+    </row>
+    <row r="25" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="O25" s="4">
+        <f>AVERAGE(O8:O16)</f>
+        <v>0.76068376068376087</v>
+      </c>
+      <c r="P25" s="4">
+        <f t="shared" ref="P25:X25" si="29">AVERAGE(P8:P16)</f>
+        <v>0.90000000000000013</v>
+      </c>
+      <c r="Q25" s="4">
+        <f t="shared" si="29"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="R25" s="4">
+        <f t="shared" si="29"/>
+        <v>0.61111111111111116</v>
+      </c>
+      <c r="S25" s="4"/>
+      <c r="T25" s="4">
+        <f t="shared" si="29"/>
+        <v>0.76666666666666672</v>
+      </c>
+      <c r="U25" s="4">
+        <f t="shared" si="29"/>
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="V25" s="4">
+        <f t="shared" si="29"/>
+        <v>0.52991452991452992</v>
+      </c>
+      <c r="W25" s="4">
+        <f t="shared" si="29"/>
+        <v>0.65</v>
+      </c>
+      <c r="X25" s="4">
+        <f t="shared" si="29"/>
+        <v>0.68913857677902624</v>
       </c>
     </row>
   </sheetData>

</xml_diff>